<commit_message>
setting up for demo
</commit_message>
<xml_diff>
--- a/com.booking/src/test/resources/test_data.xlsx
+++ b/com.booking/src/test/resources/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\SeleniumBootcamp\com.booking\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.booking\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A3D4E5-0AD3-4437-A22D-C4D1FE37D16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2DF677-8BA1-47BF-A23D-E9B41A609427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="0" windowWidth="17140" windowHeight="14320" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5DC96F64-0600-4540-8EF4-E6AE23C27A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Locations" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Assertions</t>
-  </si>
-  <si>
-    <t>Stays</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Milan</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Lisbon</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Newcastle</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Perth</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Berlin</t>
   </si>
 </sst>
 </file>
@@ -400,41 +445,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C7C825-8D82-4132-9F2A-6781F4BC04E3}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>